<commit_message>
changed visualization colors colors,documentation complete, sylwester z dwójką
</commit_message>
<xml_diff>
--- a/documents/report/test results.xlsx
+++ b/documents/report/test results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pawel\Documents\STUDIA\Semestr 3\Algorytmy Geometryczne\cwicznia\projekt\documents\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD953D1-E029-4D30-A1B0-9F52CB9F34C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB3DDEA-6E5D-4F11-8646-05F567A11B11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5496" yWindow="-108" windowWidth="11520" windowHeight="12360" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testResults20201229" sheetId="2" r:id="rId1"/>
@@ -22,10 +22,19 @@
     <definedName name="DaneZewnętrzne_1" localSheetId="0" hidden="1">testResults20201229!$A$1:$H$25</definedName>
     <definedName name="DaneZewnętrzne_1" localSheetId="1" hidden="1">'testResultsV2 (2)'!$A$1:$AS$151</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -43,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="222">
   <si>
     <t>Column1.1</t>
   </si>
@@ -706,6 +715,9 @@
   </si>
   <si>
     <t>quadTree</t>
+  </si>
+  <si>
+    <t>ms</t>
   </si>
 </sst>
 </file>
@@ -771,7 +783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -780,6 +792,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1365,7 +1379,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:G20"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2031,7 +2045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48DC013B-42DD-41E0-80DB-BB1D08F17BB7}">
   <dimension ref="A1:AS151"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
+    <sheetView topLeftCell="A77" workbookViewId="0">
       <selection activeCell="C151" sqref="A146:C151"/>
     </sheetView>
   </sheetViews>
@@ -11445,7 +11459,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:P7"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11773,8 +11787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D51333-D620-4AA3-8E0D-FFFDAB42A37F}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12322,8 +12336,14 @@
       <c r="C32" s="6" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>11</v>
       </c>
@@ -12333,8 +12353,28 @@
       <c r="C33" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33">
+        <f>1000*B33</f>
+        <v>2.141</v>
+      </c>
+      <c r="E33">
+        <f>1000*C33</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="G33" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="H33" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="I33" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>12</v>
       </c>
@@ -12344,49 +12384,113 @@
       <c r="C34" s="3">
         <v>5.1229999999999998E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="5">
-        <v>1.2394000000000001E-2</v>
-      </c>
-      <c r="C35" s="3">
-        <v>0.10231999999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" s="5">
-        <v>3.8814000000000001E-2</v>
-      </c>
-      <c r="C36" s="3">
-        <v>0.22289999999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B37" s="5">
-        <v>5.1160999999999998E-2</v>
-      </c>
-      <c r="C37" s="3">
-        <v>0.34493000000000001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="5">
-        <v>5.3348E-2</v>
-      </c>
-      <c r="C38" s="3">
-        <v>0.49941000000000002</v>
+      <c r="D34">
+        <f t="shared" ref="D34:E38" si="0">1000*B34</f>
+        <v>8.1129999999999995</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>51.23</v>
+      </c>
+      <c r="F34">
+        <v>2.8944000000000001E-2</v>
+      </c>
+      <c r="G34">
+        <v>5.9131999999999997E-2</v>
+      </c>
+      <c r="H34">
+        <v>7.3208999999999996E-2</v>
+      </c>
+      <c r="I34">
+        <v>8.2575999999999997E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="B35">
+        <v>2.8944000000000001E-2</v>
+      </c>
+      <c r="C35">
+        <v>0.13048000000000001</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>28.944000000000003</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>130.48000000000002</v>
+      </c>
+      <c r="F35">
+        <v>0.13048000000000001</v>
+      </c>
+      <c r="G35">
+        <v>0.246641</v>
+      </c>
+      <c r="H35">
+        <v>0.33201000000000003</v>
+      </c>
+      <c r="I35">
+        <v>0.53023299999999995</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="B36">
+        <v>5.9131999999999997E-2</v>
+      </c>
+      <c r="C36">
+        <v>0.246641</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>59.131999999999998</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>246.64099999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="B37">
+        <v>7.3208999999999996E-2</v>
+      </c>
+      <c r="C37">
+        <v>0.33201000000000003</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>73.209000000000003</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>332.01000000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="9">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>8.2575999999999997E-2</v>
+      </c>
+      <c r="C38">
+        <v>0.53023299999999995</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>82.575999999999993</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>530.23299999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>